<commit_message>
Added images, fixed config
</commit_message>
<xml_diff>
--- a/config/predefinedResults.xlsx
+++ b/config/predefinedResults.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="133">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -1547,7 +1547,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1723,9 @@
         <v>108</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1743,7 +1745,9 @@
         <v>108</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1763,7 +1767,9 @@
         <v>108</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,7 +1789,9 @@
         <v>108</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed report version bug and labels
</commit_message>
<xml_diff>
--- a/config/predefinedResults.xlsx
+++ b/config/predefinedResults.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="135">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -97,9 +98,6 @@
     <t>Classical-scrapie</t>
   </si>
   <si>
-    <t>INC</t>
-  </si>
-  <si>
     <t>POS</t>
   </si>
   <si>
@@ -133,9 +131,6 @@
     <t>resVal</t>
   </si>
   <si>
-    <t>BSE (Initial reactor)</t>
-  </si>
-  <si>
     <t>param desc</t>
   </si>
   <si>
@@ -163,9 +158,6 @@
     <t>Positive (other than Atypical)</t>
   </si>
   <si>
-    <t>Scrapie (Initial reactor)</t>
-  </si>
-  <si>
     <t>Atypical Scrapie</t>
   </si>
   <si>
@@ -181,9 +173,6 @@
     <t>Other Scrapie</t>
   </si>
   <si>
-    <t>CWD (Initial reactor)</t>
-  </si>
-  <si>
     <t>Other CWD</t>
   </si>
   <si>
@@ -367,9 +356,6 @@
     <t>RF-00004887-PAR$POS</t>
   </si>
   <si>
-    <t>RF-00004888-PAR$INC</t>
-  </si>
-  <si>
     <t>RF-00004889-PAR$POS</t>
   </si>
   <si>
@@ -385,9 +371,6 @@
     <t>RF-00004893-PAR$POS</t>
   </si>
   <si>
-    <t>RF-00004894-PAR$INC</t>
-  </si>
-  <si>
     <t>RF-00004895-PAR$POS</t>
   </si>
   <si>
@@ -397,9 +380,6 @@
     <t>RF-00004897-PAR$POS</t>
   </si>
   <si>
-    <t>RF-00004898-PAR$INC</t>
-  </si>
-  <si>
     <t>codici</t>
   </si>
   <si>
@@ -425,6 +405,33 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>BSE initial reactor</t>
+  </si>
+  <si>
+    <t>Scrapie initial reactor</t>
+  </si>
+  <si>
+    <t>CWD initial reactor</t>
+  </si>
+  <si>
+    <t>RF-00004884-PAR$NEG</t>
+  </si>
+  <si>
+    <t>RF-00004889-PAR$NEG</t>
+  </si>
+  <si>
+    <t>RF-00004895-PAR$NEG</t>
+  </si>
+  <si>
+    <t>RF-00004888-PAR$POS</t>
+  </si>
+  <si>
+    <t>RF-00004894-PAR$POS</t>
+  </si>
+  <si>
+    <t>RF-00004898-PAR$POS</t>
   </si>
 </sst>
 </file>
@@ -454,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +472,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -524,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -534,6 +547,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1547,7 +1565,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,25 +1585,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -1602,13 +1620,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1617,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1626,13 +1644,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1641,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1650,13 +1668,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1665,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1674,13 +1692,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1689,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1698,10 +1716,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1711,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1720,11 +1738,11 @@
         <v>6</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1733,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1742,11 +1760,11 @@
         <v>8</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1755,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -1764,11 +1782,11 @@
         <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1777,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
@@ -1786,11 +1804,11 @@
         <v>11</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="1" t="s">
-        <v>113</v>
+      <c r="G10" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1799,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1808,11 +1826,11 @@
         <v>12</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1821,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>14</v>
@@ -1830,16 +1848,16 @@
         <v>15</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1847,25 +1865,25 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1873,25 +1891,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1899,7 +1917,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>17</v>
@@ -1908,16 +1926,16 @@
         <v>22</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1925,7 +1943,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>3</v>
@@ -1934,16 +1952,16 @@
         <v>18</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>119</v>
+        <v>105</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1951,7 +1969,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>4</v>
@@ -1960,10 +1978,10 @@
         <v>12</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1973,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>14</v>
@@ -1982,14 +2000,14 @@
         <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,23 +2015,23 @@
         <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2021,23 +2039,23 @@
         <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>17</v>
@@ -2054,14 +2072,14 @@
         <v>22</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,7 +2087,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>3</v>
@@ -2078,14 +2096,14 @@
         <v>18</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="8" t="s">
-        <v>119</v>
+      <c r="G22" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2093,7 +2111,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>4</v>
@@ -2102,11 +2120,11 @@
         <v>12</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -2115,7 +2133,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>20</v>
@@ -2124,13 +2142,13 @@
         <v>19</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -2139,7 +2157,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>16</v>
@@ -2148,13 +2166,13 @@
         <v>21</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -2163,7 +2181,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>3</v>
@@ -2172,13 +2190,13 @@
         <v>18</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>123</v>
+        <v>105</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -2187,7 +2205,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>4</v>
@@ -2196,10 +2214,10 @@
         <v>12</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2209,7 +2227,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>20</v>
@@ -2218,11 +2236,11 @@
         <v>19</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -2231,20 +2249,20 @@
         <v>19</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -2253,7 +2271,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>3</v>
@@ -2262,11 +2280,11 @@
         <v>18</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="8" t="s">
-        <v>123</v>
+      <c r="G30" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -2275,7 +2293,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>4</v>
@@ -2284,11 +2302,11 @@
         <v>12</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H31" s="7"/>
     </row>
@@ -2304,14 +2322,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="3" width="34" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
@@ -2324,28 +2343,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,29 +2372,29 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>107</v>
+        <v>30</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2383,29 +2402,29 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT06A</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2413,29 +2432,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2443,29 +2462,29 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT08A</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2473,29 +2492,29 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2503,29 +2522,29 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2533,29 +2552,29 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2563,29 +2582,29 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2593,29 +2612,29 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>BSEAT12A</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>113</v>
+      <c r="H10" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2623,29 +2642,29 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>107</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2653,29 +2672,29 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT06A</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2683,29 +2702,29 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2713,29 +2732,29 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2743,29 +2762,29 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT08A</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,29 +2792,29 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2803,29 +2822,29 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" t="s">
-        <v>97</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2833,29 +2852,29 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2863,29 +2882,29 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2893,29 +2912,29 @@
         <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2923,29 +2942,29 @@
         <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>SCRAPIEAT12A</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>119</v>
+      <c r="H21" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2953,29 +2972,29 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>107</v>
+        <v>30</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2983,29 +3002,29 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT06A</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3013,29 +3032,29 @@
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3043,29 +3062,29 @@
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT08A</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3073,29 +3092,29 @@
         <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT12A</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,7 +3122,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
@@ -3113,19 +3132,19 @@
         <v>19</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3133,29 +3152,29 @@
         <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT12A</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3163,29 +3182,29 @@
         <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="str">
         <f>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</f>
         <v>CWDAT12A</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="8" t="s">
-        <v>123</v>
+      <c r="H29" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3195,4 +3214,152 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added errors checks, html table to see errors
</commit_message>
<xml_diff>
--- a/config/predefinedResults.xlsx
+++ b/config/predefinedResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="143">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -432,13 +432,37 @@
   </si>
   <si>
     <t>RF-00004898-PAR$POS</t>
+  </si>
+  <si>
+    <t>RGT</t>
+  </si>
+  <si>
+    <t>RF-00004629-PAR</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>F01.A057G</t>
+  </si>
+  <si>
+    <t>F01.A057P</t>
+  </si>
+  <si>
+    <t>sourceLabel</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Goat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +482,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -537,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -551,12 +581,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1011,6 +1075,38 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1236,37 +1332,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H31" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:H31"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="recordType" dataDxfId="21"/>
-    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="20"/>
-    <tableColumn id="2" name="sampAnAsses" dataDxfId="19"/>
-    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="18"/>
-    <tableColumn id="4" name="screening" dataDxfId="17"/>
-    <tableColumn id="8" name="confirmatory" dataDxfId="16"/>
-    <tableColumn id="5" name="discriminatory" dataDxfId="15"/>
-    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J45"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="recordType" dataDxfId="23"/>
+    <tableColumn id="9" name="source" dataDxfId="22"/>
+    <tableColumn id="10" name="sourceLabel" dataDxfId="0"/>
+    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="21"/>
+    <tableColumn id="2" name="sampAnAsses" dataDxfId="20"/>
+    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="19"/>
+    <tableColumn id="4" name="screening" dataDxfId="18"/>
+    <tableColumn id="8" name="confirmatory" dataDxfId="17"/>
+    <tableColumn id="5" name="discriminatory" dataDxfId="16"/>
+    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A1:I29"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="recordType" dataDxfId="8"/>
-    <tableColumn id="2" name="anMethtype" dataDxfId="7"/>
-    <tableColumn id="7" name="filter" dataDxfId="6">
+    <tableColumn id="1" name="recordType" dataDxfId="9"/>
+    <tableColumn id="2" name="anMethtype" dataDxfId="8"/>
+    <tableColumn id="7" name="filter" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="possible results" dataDxfId="5"/>
-    <tableColumn id="6" name="paramCode" dataDxfId="4"/>
-    <tableColumn id="4" name="param desc" dataDxfId="3"/>
-    <tableColumn id="5" name="resVal" dataDxfId="2"/>
-    <tableColumn id="8" name="codes" dataDxfId="1"/>
-    <tableColumn id="9" name="codici" dataDxfId="0"/>
+    <tableColumn id="3" name="possible results" dataDxfId="6"/>
+    <tableColumn id="6" name="paramCode" dataDxfId="5"/>
+    <tableColumn id="4" name="param desc" dataDxfId="4"/>
+    <tableColumn id="5" name="resVal" dataDxfId="3"/>
+    <tableColumn id="8" name="codes" dataDxfId="2"/>
+    <tableColumn id="9" name="codici" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1559,756 +1657,1252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="1" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="I5" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="15"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="I12" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="H15" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="H16" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="I16" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="8" t="s">
+      <c r="H18" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="G20" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="8" t="s">
+      <c r="H20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="11" t="s">
+      <c r="H22" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="E24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="I26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="15"/>
+      <c r="I28" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="G29" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="H29" s="15"/>
+      <c r="I29" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="15"/>
+      <c r="I32" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="H36" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="I36" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="H37" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="I37" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="H38" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="I38" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="G39" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="I39" s="15"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="8" t="s">
+      <c r="H40" s="15"/>
+      <c r="I40" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="8" t="s">
+      <c r="H41" s="15"/>
+      <c r="I41" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="11" t="s">
+      <c r="H42" s="15"/>
+      <c r="I42" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="F43" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="G43" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8" t="s">
+      <c r="H43" s="7"/>
+      <c r="I43" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed bseos genotyping (not not selectable)
</commit_message>
<xml_diff>
--- a/config/predefinedResults.xlsx
+++ b/config/predefinedResults.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="143">
   <si>
     <t>sampAnAsses</t>
   </si>
@@ -601,6 +601,38 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -1043,38 +1075,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -1332,39 +1332,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J44" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="A1:J44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J45" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:J45"/>
   <tableColumns count="10">
     <tableColumn id="1" name="recordType" dataDxfId="23"/>
     <tableColumn id="9" name="source" dataDxfId="22"/>
-    <tableColumn id="10" name="sourceLabel" dataDxfId="21"/>
-    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="20"/>
-    <tableColumn id="2" name="sampAnAsses" dataDxfId="19"/>
-    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="18"/>
-    <tableColumn id="4" name="screening" dataDxfId="17"/>
-    <tableColumn id="8" name="confirmatory" dataDxfId="16"/>
-    <tableColumn id="5" name="discriminatory" dataDxfId="15"/>
-    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="14"/>
+    <tableColumn id="10" name="sourceLabel" dataDxfId="0"/>
+    <tableColumn id="6" name="confirmatoryExecuted" dataDxfId="21"/>
+    <tableColumn id="2" name="sampAnAsses" dataDxfId="20"/>
+    <tableColumn id="3" name="sampAnAssesLabel" dataDxfId="19"/>
+    <tableColumn id="4" name="screening" dataDxfId="18"/>
+    <tableColumn id="8" name="confirmatory" dataDxfId="17"/>
+    <tableColumn id="5" name="discriminatory" dataDxfId="16"/>
+    <tableColumn id="7" name="genotypingBaseTerm" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I29" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A1:I29"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="recordType" dataDxfId="8"/>
-    <tableColumn id="2" name="anMethtype" dataDxfId="7"/>
-    <tableColumn id="7" name="filter" dataDxfId="6">
+    <tableColumn id="1" name="recordType" dataDxfId="9"/>
+    <tableColumn id="2" name="anMethtype" dataDxfId="8"/>
+    <tableColumn id="7" name="filter" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[recordType]],MID(Table2[[#This Row],[anMethtype]],1,5))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="possible results" dataDxfId="5"/>
-    <tableColumn id="6" name="paramCode" dataDxfId="4"/>
-    <tableColumn id="4" name="param desc" dataDxfId="3"/>
-    <tableColumn id="5" name="resVal" dataDxfId="2"/>
-    <tableColumn id="8" name="codes" dataDxfId="1"/>
-    <tableColumn id="9" name="codici" dataDxfId="0"/>
+    <tableColumn id="3" name="possible results" dataDxfId="6"/>
+    <tableColumn id="6" name="paramCode" dataDxfId="5"/>
+    <tableColumn id="4" name="param desc" dataDxfId="4"/>
+    <tableColumn id="5" name="resVal" dataDxfId="3"/>
+    <tableColumn id="8" name="codes" dataDxfId="2"/>
+    <tableColumn id="9" name="codici" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1657,13 +1657,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,7 +2875,7 @@
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
@@ -2883,6 +2883,24 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>